<commit_message>
fixed BWR systems for each generation
</commit_message>
<xml_diff>
--- a/static/data/python/site_flags.xlsx
+++ b/static/data/python/site_flags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Downloads\exam-generator\static\data\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F5B7B9-692D-41F5-BE70-E7EC8D956A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8A3E2F-47FC-49FC-8DBD-504D20970A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D21ABA90-795B-4E6D-AA7A-31E229C51A01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D21ABA90-795B-4E6D-AA7A-31E229C51A01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -666,30 +666,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1085,10 +1085,10 @@
   <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="13" ySplit="19" topLeftCell="N43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="19" topLeftCell="N42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1535,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="21">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1955,7 +1955,7 @@
         <v>46</v>
       </c>
       <c r="D25" s="21">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2550,7 +2550,7 @@
         <v>46</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2690,7 +2690,7 @@
         <v>46</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E46">
         <v>0</v>

</xml_diff>